<commit_message>
Add more graphs, and sleep
</commit_message>
<xml_diff>
--- a/lab2/Experiment 1/vDiodeSweep.xlsx
+++ b/lab2/Experiment 1/vDiodeSweep.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="16995" windowHeight="9255" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="16995" windowHeight="9255" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vDiodeSweep" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="semilog" sheetId="2" r:id="rId2"/>
+    <sheet name="incremental resistance" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Vin</t>
   </si>
@@ -34,13 +35,34 @@
   <si>
     <t>VC Characteristic</t>
   </si>
+  <si>
+    <t>Theoretical Fit</t>
+  </si>
+  <si>
+    <t>Is</t>
+  </si>
+  <si>
+    <t>Ut</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Rd - Experimental</t>
+  </si>
+  <si>
+    <t>Rd - Theoretical</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -524,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -611,7 +633,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -668,7 +689,7 @@
                   <c:y val="0.48426184880293954"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000E+00" sourceLinked="0"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -910,11 +931,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="567834816"/>
-        <c:axId val="567835392"/>
+        <c:axId val="135043264"/>
+        <c:axId val="135043840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="567834816"/>
+        <c:axId val="135043264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.25"/>
@@ -937,7 +958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -954,12 +974,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567835392"/>
+        <c:crossAx val="135043840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="567835392"/>
+        <c:axId val="135043840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +1002,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -999,7 +1018,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567834816"/>
+        <c:crossAx val="135043264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1075,7 +1094,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1099,7 +1117,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>semilog!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1118,7 +1136,11 @@
             <c:symbol val="circle"/>
             <c:size val="7"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD">
+                  <a:alpha val="38000"/>
+                </a:srgbClr>
+              </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:trendline>
@@ -1128,11 +1150,11 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14169154576298806"/>
-                  <c:y val="0.15900049556015905"/>
+                  <c:x val="0.14234055554585609"/>
+                  <c:y val="0.19901225260447072"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -1147,7 +1169,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$58:$B$91</c:f>
+              <c:f>semilog!$B$58:$B$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1258,7 +1280,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$58:$C$91</c:f>
+              <c:f>semilog!$C$58:$C$91</c:f>
               <c:numCache>
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1374,7 +1396,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>semilog!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1389,13 +1411,19 @@
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:srgbClr val="C0504D">
+                  <a:alpha val="8000"/>
+                </a:srgbClr>
+              </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$104</c:f>
+              <c:f>semilog!$D$4:$D$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -1707,7 +1735,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$104</c:f>
+              <c:f>semilog!$E$4:$E$104</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="101"/>
@@ -2013,6 +2041,266 @@
                 </c:pt>
                 <c:pt idx="100" formatCode="General">
                   <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>semilog!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical Fit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="38100">
+                <a:solidFill>
+                  <a:srgbClr val="9BBB59">
+                    <a:alpha val="54000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>semilog!$F$4:$F$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="54">
+                  <c:v>0.34673685045300001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.35481338923400002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.36307805476999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.37153522909699999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.38018939632100002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.389045144994</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.39810717055299999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.40738027780399999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.41686938347000002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.42657951880200001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.43651583224000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.44668359215100001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.45708818961499997</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.467735141287</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.47863009232300002</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.489778819368</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.50118723362700002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.51286138399100001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.52480746025000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.53703179636999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.54954087385799999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.56234132519000002</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.57543993733700005</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.58884365535600003</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.60255958607399995</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.61659500186100002</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.63095734447999996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.64565422903500003</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.66069344800800001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.67608297539200002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.69183097091900003</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.70794578438400002</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.724435960075</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.74131024130099998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>semilog!$G$4:$G$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="54">
+                  <c:v>9.7034276663767078E-9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.2950911675130341E-8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.7401868121182403E-8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.3543975190275547E-8</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.2079065266907946E-8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.4024338996846169E-8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.0864785665388727E-8</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.478441950365492E-8</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.1901974904028995E-7</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.684042845123922E-7</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.4021398682273667E-7</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.4549063297548176E-7</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.0113043807129618E-7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.3320841904171613E-7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.0823155349406689E-6</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.6122032866483864E-6</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.4239124823359375E-6</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.6790796511442807E-6</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.6387475841219039E-6</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.7286212864505971E-6</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.3649878820345978E-5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.15692501519587E-5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.4448456040326209E-5</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.5621250726639844E-5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.0815156323381801E-5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.499807106090863E-4</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.5060370534009418E-4</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.2377251925716547E-4</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7.2542460037968099E-4</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.2574471421091121E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.207759864140851E-3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.9274275586444023E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.08094828439768E-3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.2943069328907509E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2027,14 +2315,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="578929792"/>
-        <c:axId val="578886976"/>
+        <c:axId val="571781632"/>
+        <c:axId val="88473600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="578929792"/>
+        <c:axId val="571781632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.25"/>
+          <c:max val="0.76000000000000012"/>
+          <c:min val="0.29000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2078,12 +2367,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578886976"/>
+        <c:crossAx val="88473600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="578886976"/>
+        <c:axId val="88473600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2131,7 +2420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578929792"/>
+        <c:crossAx val="571781632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2142,14 +2431,719 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.791702312155548E-2"/>
-          <c:y val="0.16836684202157409"/>
-          <c:w val="0.29680111825102329"/>
-          <c:h val="0.28694040774719354"/>
+          <c:x val="0.14575060770679846"/>
+          <c:y val="0.2115771374368427"/>
+          <c:w val="0.22422760605213116"/>
+          <c:h val="0.15748027642132373"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Incremental Resistance of a Diode-Connected</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Transistor</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'incremental resistance'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rd - Experimental</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:noFill/>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD">
+                  <a:alpha val="36000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'incremental resistance'!$B$2:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1.3000000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5300000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.85E-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.33E-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8900000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.92E-8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2199999999999998E-8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.24E-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.004E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4100000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0800000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0199999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4900000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6899999999999997E-7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.02E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5829999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9500000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.2600000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8900000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5820000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6699999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.2899999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.8899999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.097E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7540000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9100000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.64E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.45E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1969999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.913E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1199999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.3400000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'incremental resistance'!$C$2:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>3511538.6956521701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2582708.1250000098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1761911.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1545386.9642857099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>859781.45631067699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>697078.92307692301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>459064.70297029702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>338896.60714285698</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>239165.91133005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>148303.17910447699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>108167.65957446799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70779.578231292398</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48395.231818181899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31039.746438746399</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19802.357015985701</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12441.019629225701</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8051.1379310345201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5171.4614718614603</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3367.5856749311101</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2109.4566610455299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1176.51204044118</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>808.55629629629402</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>515.527615384618</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>336.17477941176497</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>213.628858447487</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>124.241712802769</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>84.953092485549107</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>53.520352313167002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>34.047626106194897</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21.994407821229</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.3511292460646</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.8155809523809694</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.6434177165354296</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.7964816666666703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'incremental resistance'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rd - Theoretical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:srgbClr val="C0504D">
+                  <a:alpha val="28000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C0504D">
+                  <a:alpha val="34000"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'incremental resistance'!$B$2:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>1.3000000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5300000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.85E-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.33E-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8900000000000001E-8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.92E-8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2199999999999998E-8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.24E-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.004E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4100000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0800000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0199999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4900000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6899999999999997E-7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.02E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5829999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9500000000000003E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.2600000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8900000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5820000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6699999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.2899999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.8899999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.097E-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7540000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9100000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.64E-4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.45E-4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1969999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.913E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1199999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.3400000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'incremental resistance'!$D$2:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>2152076.923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1828562.0915032676</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1512270.2702702701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200729.6137339056</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>968062.28373702418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>713698.97959183669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>535957.85440613027</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>386422.65193370165</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>278655.37848605576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>198418.43971631204</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>134504.80769230769</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92639.072847682124</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>62309.576837416476</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41819.133034379673</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27428.431372549017</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17673.404927353127</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11190.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7082.7848101265818</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4469.169329073482</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2828.8169868554091</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1768.4576485461439</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1047.8277153558051</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>652.14452214452217</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>406.05224963715528</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>255.03190519598905</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>159.50399087799315</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96.14089347079036</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>60.295258620689651</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37.553020134228184</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>23.372598162071846</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.624673288029273</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.9669871794871785</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8285416666666672</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.8115803814713893</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="88475904"/>
+        <c:axId val="88476480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="88475904"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Current</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88476480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="88476480"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Incremental</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                  <a:t> Resistance</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88475904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.68902836322613592"/>
+          <c:y val="0.1198831910717043"/>
+          <c:w val="0.19738660934566141"/>
+          <c:h val="0.11354463045060544"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2215,16 +3209,51 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>638173</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3093,17 +4122,299 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D102"/>
+  <dimension ref="B1:H102"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C89" sqref="C56:C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
@@ -3250,7 +4561,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.141253754462</v>
       </c>
@@ -3259,7 +4570,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.144543977075</v>
       </c>
@@ -3268,7 +4579,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.14791083881700001</v>
       </c>
@@ -3277,7 +4588,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.15135612484399999</v>
       </c>
@@ -3286,7 +4597,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.154881661891</v>
       </c>
@@ -3295,7 +4606,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.15848931924599999</v>
       </c>
@@ -3304,7 +4615,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.162181009736</v>
       </c>
@@ -3313,7 +4624,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.16595869074399999</v>
       </c>
@@ -3322,7 +4633,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.169824365246</v>
       </c>
@@ -3331,7 +4642,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.17378008287499999</v>
       </c>
@@ -3340,7 +4651,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.17782794100400001</v>
       </c>
@@ -3349,7 +4660,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.181970085861</v>
       </c>
@@ -3358,7 +4669,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.186208713666</v>
       </c>
@@ -3366,8 +4677,15 @@
         <v>2.4E-9</v>
       </c>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <f>4.02159*10^(-14)</f>
+        <v>4.0215899999999998E-14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.190546071796</v>
       </c>
@@ -3375,8 +4693,19 @@
         <v>3E-9</v>
       </c>
       <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <f>3.57439*10^(1)</f>
+        <v>35.743900000000004</v>
+      </c>
+      <c r="H30">
+        <f>1/G30</f>
+        <v>2.7976801636083355E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.194984459976</v>
       </c>
@@ -3385,7 +4714,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.199526231497</v>
       </c>
@@ -4022,1265 +5351,1192 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F104"/>
+  <dimension ref="B2:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <f>4.02159*10^(-14)</f>
+        <v>4.0215899999999998E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <f>3.57439*10^(1)</f>
+        <v>35.743900000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.1</v>
       </c>
       <c r="C4" s="3">
         <v>2.7999999999999998E-9</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
+        <v>-0.01</v>
+      </c>
+      <c r="E4" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="E4">
-        <v>-0.01</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.10232929922800001</v>
       </c>
       <c r="C5" s="3">
         <v>2.7000000000000002E-9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E5" s="2">
         <v>1.17489755494E-9</v>
       </c>
-      <c r="E5">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.17489755494E-9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.10471285480500001</v>
       </c>
       <c r="C6" s="3">
         <v>2.1999999999999998E-9</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="E6" s="2">
         <v>1.3803842646000001E-9</v>
       </c>
-      <c r="E6">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.3803842646000001E-9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.107151930524</v>
       </c>
       <c r="C7" s="3">
         <v>2.1999999999999998E-9</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E7" s="2">
         <v>1.62181009736E-9</v>
       </c>
-      <c r="E7">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.62181009736E-9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.109647819614</v>
       </c>
       <c r="C8" s="3">
         <v>2.1000000000000002E-9</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E8" s="2">
         <v>1.9054607179600002E-9</v>
       </c>
-      <c r="E8">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.9054607179600002E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.11220184543</v>
       </c>
       <c r="C9" s="3">
         <v>1.6999999999999999E-9</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="E9" s="2">
         <v>2.2387211385699999E-9</v>
       </c>
-      <c r="E9">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2.2387211385699999E-9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.11481536215</v>
       </c>
       <c r="C10" s="3">
         <v>1.6999999999999999E-9</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
+        <v>0.313</v>
+      </c>
+      <c r="E10" s="2">
         <v>2.6302679919000002E-9</v>
       </c>
-      <c r="E10">
-        <v>0.313</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2.6302679919000002E-9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.11748975549399999</v>
       </c>
       <c r="C11" s="3">
         <v>2.1000000000000002E-9</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="E11" s="2">
         <v>3.0902954325099998E-9</v>
       </c>
-      <c r="E11">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="F11" s="2">
-        <v>3.0902954325099998E-9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.120226443462</v>
       </c>
       <c r="C12" s="3">
         <v>1.9000000000000001E-9</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E12" s="2">
         <v>3.6307805476999998E-9</v>
       </c>
-      <c r="E12">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3.6307805476999998E-9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.12302687708100001</v>
       </c>
       <c r="C13" s="3">
         <v>1.5E-9</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
+        <v>0.33</v>
+      </c>
+      <c r="E13" s="2">
         <v>4.2657951880200003E-9</v>
       </c>
-      <c r="E13">
-        <v>0.33</v>
-      </c>
-      <c r="F13" s="2">
-        <v>4.2657951880200003E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.12589254117900001</v>
       </c>
       <c r="C14" s="3">
         <v>2.1000000000000002E-9</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="E14" s="2">
         <v>5.0118723362699999E-9</v>
       </c>
-      <c r="E14">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="F14" s="2">
-        <v>5.0118723362699999E-9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.128824955169</v>
       </c>
       <c r="C15" s="3">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="E15" s="2">
         <v>5.8884365535599998E-9</v>
       </c>
-      <c r="E15">
-        <v>0.34100000000000003</v>
-      </c>
-      <c r="F15" s="2">
-        <v>5.8884365535599998E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.131825673856</v>
       </c>
       <c r="C16" s="3">
         <v>1.8E-9</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="E16" s="2">
         <v>6.9183097091900004E-9</v>
       </c>
-      <c r="E16">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="F16" s="2">
-        <v>6.9183097091900004E-9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.13489628825899999</v>
       </c>
       <c r="C17" s="3">
         <v>1.5E-9</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="E17" s="2">
         <v>8.1283051616400001E-9</v>
       </c>
-      <c r="E17">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="F17" s="2">
-        <v>8.1283051616400001E-9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.13803842646</v>
       </c>
       <c r="C18" s="3">
         <v>1.5E-9</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="E18" s="2">
         <v>9.5499258602099993E-9</v>
       </c>
-      <c r="E18">
-        <v>0.35499999999999998</v>
-      </c>
-      <c r="F18" s="2">
-        <v>9.5499258602099993E-9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.141253754462</v>
       </c>
       <c r="C19" s="3">
         <v>1.9000000000000001E-9</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
+        <v>0.36</v>
+      </c>
+      <c r="E19" s="2">
         <v>1.1220184543E-8</v>
       </c>
-      <c r="E19">
-        <v>0.36</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1.1220184543E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.144543977075</v>
       </c>
       <c r="C20" s="3">
         <v>2.1000000000000002E-9</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="E20" s="2">
         <v>1.3182567385600001E-8</v>
       </c>
-      <c r="E20">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1.3182567385600001E-8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.14791083881700001</v>
       </c>
       <c r="C21" s="3">
         <v>1.8E-9</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="E21" s="2">
         <v>1.5488166189099999E-8</v>
       </c>
-      <c r="E21">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1.5488166189099999E-8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.15135612484399999</v>
       </c>
       <c r="C22" s="3">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
+        <v>0.373</v>
+      </c>
+      <c r="E22" s="2">
         <v>1.8197008586100001E-8</v>
       </c>
-      <c r="E22">
-        <v>0.373</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1.8197008586100001E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.154881661891</v>
       </c>
       <c r="C23" s="3">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
+        <v>0.377</v>
+      </c>
+      <c r="E23" s="2">
         <v>2.1379620895000001E-8</v>
       </c>
-      <c r="E23">
-        <v>0.377</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2.1379620895000001E-8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.15848931924599999</v>
       </c>
       <c r="C24" s="3">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="E24" s="2">
         <v>2.51188643151E-8</v>
       </c>
-      <c r="E24">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2.51188643151E-8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.162181009736</v>
       </c>
       <c r="C25" s="3">
         <v>2.4E-9</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E25" s="2">
         <v>2.9512092266699999E-8</v>
       </c>
-      <c r="E25">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2.9512092266699999E-8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.16595869074399999</v>
       </c>
       <c r="C26" s="3">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26">
+        <v>0.39</v>
+      </c>
+      <c r="E26" s="2">
         <v>3.4673685045300002E-8</v>
       </c>
-      <c r="E26">
-        <v>0.39</v>
-      </c>
-      <c r="F26" s="2">
-        <v>3.4673685045300002E-8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.169824365246</v>
       </c>
       <c r="C27" s="3">
         <v>2.2999999999999999E-9</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="E27" s="2">
         <v>4.0738027780399998E-8</v>
       </c>
-      <c r="E27">
-        <v>0.39400000000000002</v>
-      </c>
-      <c r="F27" s="2">
-        <v>4.0738027780399998E-8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.17378008287499999</v>
       </c>
       <c r="C28" s="3">
         <v>3E-9</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E28" s="2">
         <v>4.7863009232299999E-8</v>
       </c>
-      <c r="E28">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="F28" s="2">
-        <v>4.7863009232299999E-8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.17782794100400001</v>
       </c>
       <c r="C29" s="3">
         <v>2.6000000000000001E-9</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="E29" s="2">
         <v>5.6234132518999998E-8</v>
       </c>
-      <c r="E29">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="F29" s="2">
-        <v>5.6234132518999998E-8</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.181970085861</v>
       </c>
       <c r="C30" s="3">
         <v>2.6000000000000001E-9</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="E30" s="2">
         <v>6.6069344800799994E-8</v>
       </c>
-      <c r="E30">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="F30" s="2">
-        <v>6.6069344800799994E-8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.186208713666</v>
       </c>
       <c r="C31" s="3">
         <v>2.4E-9</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="E31" s="2">
         <v>7.7624711662899994E-8</v>
       </c>
-      <c r="E31">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="F31" s="2">
-        <v>7.7624711662899994E-8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.190546071796</v>
       </c>
       <c r="C32" s="3">
         <v>3E-9</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="E32" s="2">
         <v>9.1201083935600003E-8</v>
       </c>
-      <c r="E32">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="F32" s="2">
-        <v>9.1201083935600003E-8</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.194984459976</v>
       </c>
       <c r="C33" s="3">
         <v>2.8999999999999999E-9</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E33" s="2">
         <v>1.07151930524E-7</v>
       </c>
-      <c r="E33">
-        <v>0.41899999999999998</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1.07151930524E-7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.199526231497</v>
       </c>
       <c r="C34" s="3">
         <v>3.1E-9</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="E34" s="2">
         <v>1.2589254117900001E-7</v>
       </c>
-      <c r="E34">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1.2589254117900001E-7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.20417379446700001</v>
       </c>
       <c r="C35" s="3">
         <v>3.4999999999999999E-9</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="E35" s="2">
         <v>1.4791083881699999E-7</v>
       </c>
-      <c r="E35">
-        <v>0.42799999999999999</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1.4791083881699999E-7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.20892961308499999</v>
       </c>
       <c r="C36" s="3">
         <v>3.8000000000000001E-9</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36">
+        <v>0.432</v>
+      </c>
+      <c r="E36" s="2">
         <v>1.7378008287500001E-7</v>
       </c>
-      <c r="E36">
-        <v>0.432</v>
-      </c>
-      <c r="F36" s="2">
-        <v>1.7378008287500001E-7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.21379620895000001</v>
       </c>
       <c r="C37" s="3">
         <v>3.8000000000000001E-9</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37">
+        <v>0.435</v>
+      </c>
+      <c r="E37" s="2">
         <v>2.04173794467E-7</v>
       </c>
-      <c r="E37">
-        <v>0.435</v>
-      </c>
-      <c r="F37" s="2">
-        <v>2.04173794467E-7</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.218776162395</v>
       </c>
       <c r="C38" s="3">
         <v>4.2000000000000004E-9</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38">
+        <v>0.44</v>
+      </c>
+      <c r="E38" s="2">
         <v>2.3988329190200001E-7</v>
       </c>
-      <c r="E38">
-        <v>0.44</v>
-      </c>
-      <c r="F38" s="2">
-        <v>2.3988329190200001E-7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.22387211385700001</v>
       </c>
       <c r="C39" s="3">
         <v>3.9000000000000002E-9</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="E39" s="2">
         <v>2.8183829312600001E-7</v>
       </c>
-      <c r="E39">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="F39" s="2">
-        <v>2.8183829312600001E-7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.229086765277</v>
       </c>
       <c r="C40" s="3">
         <v>4.1000000000000003E-9</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="E40" s="2">
         <v>3.3113112148300002E-7</v>
       </c>
-      <c r="E40">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="F40" s="2">
-        <v>3.3113112148300002E-7</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.234422881532</v>
       </c>
       <c r="C41" s="3">
         <v>4.3999999999999997E-9</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="E41" s="2">
         <v>3.8904514499400001E-7</v>
       </c>
-      <c r="E41">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="F41" s="2">
-        <v>3.8904514499400001E-7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>0.239883291902</v>
       </c>
       <c r="C42" s="3">
         <v>4.5999999999999998E-9</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="E42" s="2">
         <v>4.5708818961499999E-7</v>
       </c>
-      <c r="E42">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="F42" s="2">
-        <v>4.5708818961499999E-7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.24547089156900001</v>
       </c>
       <c r="C43" s="3">
         <v>4.2000000000000004E-9</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="E43" s="2">
         <v>5.3703179637000002E-7</v>
       </c>
-      <c r="E43">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="F43" s="2">
-        <v>5.3703179637000002E-7</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.25118864315099998</v>
       </c>
       <c r="C44" s="3">
         <v>4.9E-9</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E44" s="2">
         <v>6.3095734448000005E-7</v>
       </c>
-      <c r="E44">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="F44" s="2">
-        <v>6.3095734448000005E-7</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>0.25703957827700002</v>
       </c>
       <c r="C45" s="3">
         <v>5.1000000000000002E-9</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="E45" s="2">
         <v>7.4131024130100003E-7</v>
       </c>
-      <c r="E45">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="F45" s="2">
-        <v>7.4131024130100003E-7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.26302679918999999</v>
       </c>
       <c r="C46" s="3">
         <v>5.1000000000000002E-9</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="E46" s="2">
         <v>8.7096358995599998E-7</v>
       </c>
-      <c r="E46">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="F46" s="2">
-        <v>8.7096358995599998E-7</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>0.26915348039300002</v>
       </c>
       <c r="C47" s="3">
         <v>5.4999999999999996E-9</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="E47" s="2">
         <v>1.0232929922800001E-6</v>
       </c>
-      <c r="E47">
-        <v>0.47799999999999998</v>
-      </c>
-      <c r="F47" s="2">
-        <v>1.0232929922800001E-6</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>0.27542287033399998</v>
       </c>
       <c r="C48" s="3">
         <v>5.3000000000000003E-9</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="E48" s="2">
         <v>1.20226443462E-6</v>
       </c>
-      <c r="E48">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="F48" s="2">
-        <v>1.20226443462E-6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.28183829312600001</v>
       </c>
       <c r="C49" s="3">
         <v>5.4999999999999996E-9</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="E49" s="2">
         <v>1.41253754462E-6</v>
       </c>
-      <c r="E49">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="F49" s="2">
-        <v>1.41253754462E-6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.28840315031300001</v>
       </c>
       <c r="C50" s="3">
         <v>6.2000000000000001E-9</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="E50" s="2">
         <v>1.6595869074399999E-6</v>
       </c>
-      <c r="E50">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="F50" s="2">
-        <v>1.6595869074399999E-6</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0.29512092266700002</v>
       </c>
       <c r="C51" s="3">
         <v>6.3000000000000002E-9</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51">
+        <v>0.495</v>
+      </c>
+      <c r="E51" s="2">
         <v>1.9498445997599999E-6</v>
       </c>
-      <c r="E51">
-        <v>0.495</v>
-      </c>
-      <c r="F51" s="2">
-        <v>1.9498445997599999E-6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0.30199517203999998</v>
       </c>
       <c r="C52" s="3">
         <v>6.5000000000000003E-9</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52">
+        <v>0.498</v>
+      </c>
+      <c r="E52" s="2">
         <v>2.2908676527699999E-6</v>
       </c>
-      <c r="E52">
-        <v>0.498</v>
-      </c>
-      <c r="F52" s="2">
-        <v>2.2908676527699999E-6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.30902954325100002</v>
       </c>
       <c r="C53" s="3">
         <v>6.9999999999999998E-9</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53">
+        <v>0.503</v>
+      </c>
+      <c r="E53" s="2">
         <v>2.69153480393E-6</v>
       </c>
-      <c r="E53">
-        <v>0.503</v>
-      </c>
-      <c r="F53" s="2">
-        <v>2.69153480393E-6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.31622776601699998</v>
       </c>
       <c r="C54" s="3">
         <v>7.8999999999999996E-9</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E54" s="2">
         <v>3.16227766017E-6</v>
       </c>
-      <c r="E54">
-        <v>0.50700000000000001</v>
-      </c>
-      <c r="F54" s="2">
-        <v>3.16227766017E-6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.32359365692999997</v>
       </c>
       <c r="C55" s="3">
         <v>8.7999999999999994E-9</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="E55" s="2">
         <v>3.7153522909700001E-6</v>
       </c>
-      <c r="E55">
-        <v>0.51100000000000001</v>
-      </c>
-      <c r="F55" s="2">
-        <v>3.7153522909700001E-6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>0.331131121483</v>
       </c>
       <c r="C56" s="3">
         <v>9.3999999999999998E-9</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="E56" s="2">
         <v>4.3651583223999998E-6</v>
       </c>
-      <c r="E56">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="F56" s="2">
-        <v>4.3651583223999998E-6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0.33884415613899999</v>
       </c>
       <c r="C57" s="3">
         <v>1.14E-8</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57">
+        <v>0.52</v>
+      </c>
+      <c r="E57" s="2">
         <v>5.1286138399099999E-6</v>
       </c>
-      <c r="E57">
-        <v>0.52</v>
-      </c>
-      <c r="F57" s="2">
-        <v>5.1286138399099999E-6</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0.34673685045300001</v>
       </c>
       <c r="C58" s="3">
         <v>1.3000000000000001E-8</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="E58" s="2">
         <v>6.0255958607400004E-6</v>
       </c>
-      <c r="E58">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="F58" s="2">
-        <v>6.0255958607400004E-6</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>0.34673685045300001</v>
+      </c>
+      <c r="G58">
+        <f t="shared" ref="G58:G68" si="0">$I$2*EXP(F58*($I$3))</f>
+        <v>9.7034276663767078E-9</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0.35481338923400002</v>
       </c>
       <c r="C59" s="3">
         <v>1.5300000000000001E-8</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="E59" s="2">
         <v>7.0794578438400003E-6</v>
       </c>
-      <c r="E59">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="F59" s="2">
-        <v>7.0794578438400003E-6</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>0.35481338923400002</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>1.2950911675130341E-8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>0.36307805476999999</v>
       </c>
       <c r="C60" s="3">
         <v>1.85E-8</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="E60" s="2">
         <v>8.3176377110299993E-6</v>
       </c>
-      <c r="E60">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="F60" s="2">
-        <v>8.3176377110299993E-6</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>0.36307805476999999</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>1.7401868121182403E-8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>0.37153522909699999</v>
       </c>
       <c r="C61" s="3">
         <v>2.33E-8</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="E61" s="2">
         <v>9.7723722095599999E-6</v>
       </c>
-      <c r="E61">
-        <v>0.53700000000000003</v>
-      </c>
-      <c r="F61" s="2">
-        <v>9.7723722095599999E-6</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>0.37153522909699999</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>2.3543975190275547E-8</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>0.38018939632100002</v>
       </c>
       <c r="C62" s="3">
         <v>2.8900000000000001E-8</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="E62" s="2">
         <v>1.1481536215E-5</v>
       </c>
-      <c r="E62">
-        <v>0.54100000000000004</v>
-      </c>
-      <c r="F62" s="2">
-        <v>1.1481536215E-5</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>0.38018939632100002</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>3.2079065266907946E-8</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>0.389045144994</v>
       </c>
       <c r="C63" s="3">
         <v>3.92E-8</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="E63" s="2">
         <v>1.3489628825900001E-5</v>
       </c>
-      <c r="E63">
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="F63" s="2">
-        <v>1.3489628825900001E-5</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>0.389045144994</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>4.4024338996846169E-8</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>0.39810717055299999</v>
       </c>
       <c r="C64" s="3">
         <v>5.2199999999999998E-8</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="E64" s="2">
         <v>1.5848931924600001E-5</v>
       </c>
-      <c r="E64">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="F64" s="2">
-        <v>1.5848931924600001E-5</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>0.39810717055299999</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>6.0864785665388727E-8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>0.40738027780399999</v>
       </c>
       <c r="C65" s="3">
         <v>7.24E-8</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="E65" s="2">
         <v>1.86208713666E-5</v>
       </c>
-      <c r="E65">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="F65" s="2">
-        <v>1.86208713666E-5</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>0.40738027780399999</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>8.478441950365492E-8</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>0.41686938347000002</v>
       </c>
       <c r="C66" s="3">
         <v>1.004E-7</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="E66" s="2">
         <v>2.1877616239500002E-5</v>
       </c>
-      <c r="E66">
-        <v>0.55700000000000005</v>
-      </c>
-      <c r="F66" s="2">
-        <v>2.1877616239500002E-5</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>0.41686938347000002</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>1.1901974904028995E-7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>0.42657951880200001</v>
       </c>
       <c r="C67" s="3">
         <v>1.4100000000000001E-7</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="E67" s="2">
         <v>2.5703957827699999E-5</v>
       </c>
-      <c r="E67">
-        <v>0.56200000000000006</v>
-      </c>
-      <c r="F67" s="2">
-        <v>2.5703957827699999E-5</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>0.42657951880200001</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="0"/>
+        <v>1.684042845123922E-7</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>0.43651583224000001</v>
       </c>
       <c r="C68" s="3">
         <v>2.0800000000000001E-7</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="E68" s="2">
         <v>3.0199517203999999E-5</v>
       </c>
-      <c r="E68">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="F68" s="2">
-        <v>3.0199517203999999E-5</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>0.43651583224000001</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="0"/>
+        <v>2.4021398682273667E-7</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>0.44668359215100001</v>
       </c>
       <c r="C69" s="3">
         <v>3.0199999999999998E-7</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="E69" s="2">
         <v>3.54813389234E-5</v>
       </c>
-      <c r="E69">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="F69" s="2">
-        <v>3.54813389234E-5</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>0.44668359215100001</v>
+      </c>
+      <c r="G69">
+        <f t="shared" ref="G69:G91" si="1">$I$2*EXP(F69*($I$3))</f>
+        <v>3.4549063297548176E-7</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>0.45708818961499997</v>
       </c>
       <c r="C70" s="3">
         <v>4.4900000000000001E-7</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="E70" s="2">
         <v>4.1686938347000003E-5</v>
       </c>
-      <c r="E70">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F70" s="2">
-        <v>4.1686938347000003E-5</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>0.45708818961499997</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="1"/>
+        <v>5.0113043807129618E-7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>0.467735141287</v>
       </c>
       <c r="C71" s="3">
         <v>6.6899999999999997E-7</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E71" s="2">
         <v>4.89778819368E-5</v>
       </c>
-      <c r="E71">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F71" s="2">
-        <v>4.89778819368E-5</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>0.467735141287</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="1"/>
+        <v>7.3320841904171613E-7</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>0.47863009232300002</v>
       </c>
       <c r="C72" s="3">
         <v>1.02E-6</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E72" s="2">
         <v>5.7543993733699997E-5</v>
       </c>
-      <c r="E72">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="F72" s="2">
-        <v>5.7543993733699997E-5</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>0.47863009232300002</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="1"/>
+        <v>1.0823155349406689E-6</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>0.489778819368</v>
       </c>
       <c r="C73" s="3">
         <v>1.5829999999999999E-6</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="E73" s="2">
         <v>6.7608297539200005E-5</v>
       </c>
-      <c r="E73">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="F73" s="2">
-        <v>6.7608297539200005E-5</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>0.489778819368</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="1"/>
+        <v>1.6122032866483864E-6</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>0.50118723362700002</v>
       </c>
       <c r="C74" s="3">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="E74" s="2">
         <v>7.9432823472400004E-5</v>
       </c>
-      <c r="E74">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="F74" s="2">
-        <v>7.9432823472400004E-5</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>0.50118723362700002</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>2.4239124823359375E-6</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>0.51286138399100001</v>
       </c>
       <c r="C75" s="3">
         <v>3.9500000000000003E-6</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="E75" s="2">
         <v>9.3325430079699994E-5</v>
       </c>
-      <c r="E75">
-        <v>0.59799999999999998</v>
-      </c>
-      <c r="F75" s="2">
-        <v>9.3325430079699994E-5</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>0.51286138399100001</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="1"/>
+        <v>3.6790796511442807E-6</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>0.52480746025000002</v>
       </c>
@@ -5288,16 +6544,20 @@
         <v>6.2600000000000002E-6</v>
       </c>
       <c r="D76">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="E76">
         <v>1.09647819614E-4</v>
       </c>
-      <c r="E76">
-        <v>0.60299999999999998</v>
-      </c>
       <c r="F76">
-        <v>1.09647819614E-4</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.52480746025000002</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="1"/>
+        <v>5.6387475841219039E-6</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>0.53703179636999998</v>
       </c>
@@ -5305,16 +6565,20 @@
         <v>9.8900000000000002E-6</v>
       </c>
       <c r="D77">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="E77">
         <v>1.28824955169E-4</v>
       </c>
-      <c r="E77">
-        <v>0.60699999999999998</v>
-      </c>
       <c r="F77">
-        <v>1.28824955169E-4</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.53703179636999998</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="1"/>
+        <v>8.7286212864505971E-6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>0.54954087385799999</v>
       </c>
@@ -5322,16 +6586,20 @@
         <v>1.5820000000000001E-5</v>
       </c>
       <c r="D78">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="E78">
         <v>1.51356124844E-4</v>
       </c>
-      <c r="E78">
-        <v>0.61199999999999999</v>
-      </c>
       <c r="F78">
-        <v>1.51356124844E-4</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.54954087385799999</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="1"/>
+        <v>1.3649878820345978E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>0.56234132519000002</v>
       </c>
@@ -5339,16 +6607,20 @@
         <v>2.6699999999999998E-5</v>
       </c>
       <c r="D79">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E79">
         <v>1.7782794100400001E-4</v>
       </c>
-      <c r="E79">
-        <v>0.61699999999999999</v>
-      </c>
       <c r="F79">
-        <v>1.7782794100400001E-4</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.56234132519000002</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="1"/>
+        <v>2.15692501519587E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>0.57543993733700005</v>
       </c>
@@ -5356,16 +6628,20 @@
         <v>4.2899999999999999E-5</v>
       </c>
       <c r="D80">
+        <v>0.621</v>
+      </c>
+      <c r="E80">
         <v>2.0892961308500001E-4</v>
       </c>
-      <c r="E80">
-        <v>0.621</v>
-      </c>
       <c r="F80">
-        <v>2.0892961308500001E-4</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.57543993733700005</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="1"/>
+        <v>3.4448456040326209E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>0.58884365535600003</v>
       </c>
@@ -5373,16 +6649,20 @@
         <v>6.8899999999999994E-5</v>
       </c>
       <c r="D81">
+        <v>0.626</v>
+      </c>
+      <c r="E81">
         <v>2.4547089156900002E-4</v>
       </c>
-      <c r="E81">
-        <v>0.626</v>
-      </c>
       <c r="F81">
-        <v>2.4547089156900002E-4</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.58884365535600003</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="1"/>
+        <v>5.5621250726639844E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>0.60255958607399995</v>
       </c>
@@ -5390,16 +6670,20 @@
         <v>1.097E-4</v>
       </c>
       <c r="D82">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="E82">
         <v>2.8840315031300001E-4</v>
       </c>
-      <c r="E82">
-        <v>0.63100000000000001</v>
-      </c>
       <c r="F82">
-        <v>2.8840315031300001E-4</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.60255958607399995</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="1"/>
+        <v>9.0815156323381801E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>0.61659500186100002</v>
       </c>
@@ -5407,16 +6691,20 @@
         <v>1.7540000000000001E-4</v>
       </c>
       <c r="D83">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="E83">
         <v>3.3884415613899999E-4</v>
       </c>
-      <c r="E83">
-        <v>0.63600000000000001</v>
-      </c>
       <c r="F83">
-        <v>3.3884415613899999E-4</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.61659500186100002</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="1"/>
+        <v>1.499807106090863E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>0.63095734447999996</v>
       </c>
@@ -5424,16 +6712,20 @@
         <v>2.9100000000000003E-4</v>
       </c>
       <c r="D84">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="E84">
         <v>3.9810717055299997E-4</v>
       </c>
-      <c r="E84">
-        <v>0.64100000000000001</v>
-      </c>
       <c r="F84">
-        <v>3.9810717055299997E-4</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.63095734447999996</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="1"/>
+        <v>2.5060370534009418E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>0.64565422903500003</v>
       </c>
@@ -5441,16 +6733,20 @@
         <v>4.64E-4</v>
       </c>
       <c r="D85">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="E85">
         <v>4.67735141287E-4</v>
       </c>
-      <c r="E85">
-        <v>0.64600000000000002</v>
-      </c>
       <c r="F85">
-        <v>4.67735141287E-4</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.64565422903500003</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="1"/>
+        <v>4.2377251925716547E-4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>0.66069344800800001</v>
       </c>
@@ -5458,16 +6754,20 @@
         <v>7.45E-4</v>
       </c>
       <c r="D86">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="E86">
         <v>5.4954087385800001E-4</v>
       </c>
-      <c r="E86">
-        <v>0.65200000000000002</v>
-      </c>
       <c r="F86">
-        <v>5.4954087385800001E-4</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.66069344800800001</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="1"/>
+        <v>7.2542460037968099E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>0.67608297539200002</v>
       </c>
@@ -5475,16 +6775,20 @@
         <v>1.1969999999999999E-3</v>
       </c>
       <c r="D87">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="E87">
         <v>6.4565422903500001E-4</v>
       </c>
-      <c r="E87">
-        <v>0.65700000000000003</v>
-      </c>
       <c r="F87">
-        <v>6.4565422903500001E-4</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.67608297539200002</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="1"/>
+        <v>1.2574471421091121E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>0.69183097091900003</v>
       </c>
@@ -5492,16 +6796,20 @@
         <v>1.913E-3</v>
       </c>
       <c r="D88">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="E88">
         <v>7.5857757502899997E-4</v>
       </c>
-      <c r="E88">
-        <v>0.66200000000000003</v>
-      </c>
       <c r="F88">
-        <v>7.5857757502899997E-4</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.69183097091900003</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="1"/>
+        <v>2.207759864140851E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>0.70794578438400002</v>
       </c>
@@ -5509,16 +6817,20 @@
         <v>3.1199999999999999E-3</v>
       </c>
       <c r="D89">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="E89">
         <v>8.9125093813399996E-4</v>
       </c>
-      <c r="E89">
-        <v>0.66700000000000004</v>
-      </c>
       <c r="F89">
-        <v>8.9125093813399996E-4</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.70794578438400002</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="1"/>
+        <v>3.9274275586444023E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>0.724435960075</v>
       </c>
@@ -5526,16 +6838,20 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="D90">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="E90">
         <v>1.0471285480499999E-3</v>
       </c>
-      <c r="E90">
-        <v>0.67200000000000004</v>
-      </c>
       <c r="F90">
-        <v>1.0471285480499999E-3</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.724435960075</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="1"/>
+        <v>7.08094828439768E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>0.74131024130099998</v>
       </c>
@@ -5543,16 +6859,20 @@
         <v>7.3400000000000002E-3</v>
       </c>
       <c r="D91">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="E91">
         <v>1.2302687708100001E-3</v>
       </c>
-      <c r="E91">
-        <v>0.67800000000000005</v>
-      </c>
       <c r="F91">
-        <v>1.2302687708100001E-3</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.74131024130099998</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="1"/>
+        <v>1.2943069328907509E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>0.75857757502900003</v>
       </c>
@@ -5560,16 +6880,13 @@
         <v>1.094E-2</v>
       </c>
       <c r="D92">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E92">
         <v>1.44543977075E-3</v>
       </c>
-      <c r="E92">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="F92">
-        <v>1.44543977075E-3</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>0.77624711662900003</v>
       </c>
@@ -5577,16 +6894,13 @@
         <v>1.6150000000000001E-2</v>
       </c>
       <c r="D93">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="E93">
         <v>1.69824365246E-3</v>
       </c>
-      <c r="E93">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="F93">
-        <v>1.69824365246E-3</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>0.79432823472400005</v>
       </c>
@@ -5594,16 +6908,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D94">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="E94">
         <v>1.99526231497E-3</v>
       </c>
-      <c r="E94">
-        <v>0.69399999999999995</v>
-      </c>
-      <c r="F94">
-        <v>1.99526231497E-3</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>0.81283051616400004</v>
       </c>
@@ -5611,16 +6922,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D95">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="E95">
         <v>2.3442288153200002E-3</v>
       </c>
-      <c r="E95">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="F95">
-        <v>2.3442288153200002E-3</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>0.83176377110300004</v>
       </c>
@@ -5628,16 +6936,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D96">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="E96">
         <v>2.75422870334E-3</v>
       </c>
-      <c r="E96">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="F96">
-        <v>2.75422870334E-3</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>0.85113803820199996</v>
       </c>
@@ -5645,16 +6950,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D97">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="E97">
         <v>3.2359365693E-3</v>
       </c>
-      <c r="E97">
-        <v>0.71099999999999997</v>
-      </c>
-      <c r="F97">
-        <v>3.2359365693E-3</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0.87096358995599998</v>
       </c>
@@ -5662,16 +6964,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D98">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="E98">
         <v>3.8018939632099998E-3</v>
       </c>
-      <c r="E98">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="F98">
-        <v>3.8018939632099998E-3</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0.89125093813400003</v>
       </c>
@@ -5679,16 +6978,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D99">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="E99">
         <v>4.46683592151E-3</v>
       </c>
-      <c r="E99">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="F99">
-        <v>4.46683592151E-3</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0.91201083935600002</v>
       </c>
@@ -5696,16 +6992,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D100">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="E100">
         <v>5.2480746024999997E-3</v>
       </c>
-      <c r="E100">
-        <v>0.72899999999999998</v>
-      </c>
-      <c r="F100">
-        <v>5.2480746024999997E-3</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0.933254300797</v>
       </c>
@@ -5713,16 +7006,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D101">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="E101">
         <v>6.1659500186099997E-3</v>
       </c>
-      <c r="E101">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="F101">
-        <v>6.1659500186099997E-3</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>0.95499258602100001</v>
       </c>
@@ -5730,16 +7020,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D102">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="E102">
         <v>7.2443596007499998E-3</v>
       </c>
-      <c r="E102">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="F102">
-        <v>7.2443596007499998E-3</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>0.97723722095599996</v>
       </c>
@@ -5747,16 +7034,13 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D103">
+        <v>0.748</v>
+      </c>
+      <c r="E103">
         <v>8.5113803820199996E-3</v>
       </c>
-      <c r="E103">
-        <v>0.748</v>
-      </c>
-      <c r="F103">
-        <v>8.5113803820199996E-3</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>1</v>
       </c>
@@ -5764,13 +7048,554 @@
         <v>2.0619999999999999E-2</v>
       </c>
       <c r="D104">
+        <v>0.754</v>
+      </c>
+      <c r="E104">
         <v>0.01</v>
       </c>
-      <c r="E104">
-        <v>0.754</v>
-      </c>
-      <c r="F104">
-        <v>0.01</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.34673685045300001</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.3000000000000001E-8</v>
+      </c>
+      <c r="C2">
+        <v>3511538.6956521701</v>
+      </c>
+      <c r="D2" s="3">
+        <f>0.027977/B2</f>
+        <v>2152076.923076923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.35481338923400002</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.5300000000000001E-8</v>
+      </c>
+      <c r="C3">
+        <v>2582708.1250000098</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D35" si="0">0.027977/B3</f>
+        <v>1828562.0915032676</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.36307805476999999</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.85E-8</v>
+      </c>
+      <c r="C4">
+        <v>1761911.25</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>1512270.2702702701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.37153522909699999</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2.33E-8</v>
+      </c>
+      <c r="C5">
+        <v>1545386.9642857099</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>1200729.6137339056</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.38018939632100002</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.8900000000000001E-8</v>
+      </c>
+      <c r="C6">
+        <v>859781.45631067699</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>968062.28373702418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.389045144994</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3.92E-8</v>
+      </c>
+      <c r="C7">
+        <v>697078.92307692301</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>713698.97959183669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.39810717055299999</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5.2199999999999998E-8</v>
+      </c>
+      <c r="C8">
+        <v>459064.70297029702</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>535957.85440613027</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.40738027780399999</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7.24E-8</v>
+      </c>
+      <c r="C9">
+        <v>338896.60714285698</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>386422.65193370165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.41686938347000002</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.004E-7</v>
+      </c>
+      <c r="C10">
+        <v>239165.91133005</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>278655.37848605576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.42657951880200001</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.4100000000000001E-7</v>
+      </c>
+      <c r="C11">
+        <v>148303.17910447699</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>198418.43971631204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.43651583224000001</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2.0800000000000001E-7</v>
+      </c>
+      <c r="C12">
+        <v>108167.65957446799</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>134504.80769230769</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.44668359215100001</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3.0199999999999998E-7</v>
+      </c>
+      <c r="C13">
+        <v>70779.578231292398</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>92639.072847682124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.45708818961499997</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4.4900000000000001E-7</v>
+      </c>
+      <c r="C14">
+        <v>48395.231818181899</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>62309.576837416476</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.467735141287</v>
+      </c>
+      <c r="B15" s="3">
+        <v>6.6899999999999997E-7</v>
+      </c>
+      <c r="C15">
+        <v>31039.746438746399</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>41819.133034379673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.47863009232300002</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.02E-6</v>
+      </c>
+      <c r="C16">
+        <v>19802.357015985701</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>27428.431372549017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.489778819368</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.5829999999999999E-6</v>
+      </c>
+      <c r="C17">
+        <v>12441.019629225701</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>17673.404927353127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.50118723362700002</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2.5000000000000002E-6</v>
+      </c>
+      <c r="C18">
+        <v>8051.1379310345201</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>11190.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.51286138399100001</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3.9500000000000003E-6</v>
+      </c>
+      <c r="C19">
+        <v>5171.4614718614603</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>7082.7848101265818</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.52480746025000002</v>
+      </c>
+      <c r="B20" s="3">
+        <v>6.2600000000000002E-6</v>
+      </c>
+      <c r="C20">
+        <v>3367.5856749311101</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>4469.169329073482</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.53703179636999998</v>
+      </c>
+      <c r="B21" s="3">
+        <v>9.8900000000000002E-6</v>
+      </c>
+      <c r="C21">
+        <v>2109.4566610455299</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>2828.8169868554091</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.54954087385799999</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.5820000000000001E-5</v>
+      </c>
+      <c r="C22">
+        <v>1176.51204044118</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>1768.4576485461439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.56234132519000002</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2.6699999999999998E-5</v>
+      </c>
+      <c r="C23">
+        <v>808.55629629629402</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>1047.8277153558051</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.57543993733700005</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4.2899999999999999E-5</v>
+      </c>
+      <c r="C24">
+        <v>515.527615384618</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>652.14452214452217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.58884365535600003</v>
+      </c>
+      <c r="B25" s="3">
+        <v>6.8899999999999994E-5</v>
+      </c>
+      <c r="C25">
+        <v>336.17477941176497</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>406.05224963715528</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.60255958607399995</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.097E-4</v>
+      </c>
+      <c r="C26">
+        <v>213.628858447487</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>255.03190519598905</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.61659500186100002</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1.7540000000000001E-4</v>
+      </c>
+      <c r="C27">
+        <v>124.241712802769</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>159.50399087799315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.63095734447999996</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2.9100000000000003E-4</v>
+      </c>
+      <c r="C28">
+        <v>84.953092485549107</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>96.14089347079036</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.64565422903500003</v>
+      </c>
+      <c r="B29" s="3">
+        <v>4.64E-4</v>
+      </c>
+      <c r="C29">
+        <v>53.520352313167002</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>60.295258620689651</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.66069344800800001</v>
+      </c>
+      <c r="B30" s="3">
+        <v>7.45E-4</v>
+      </c>
+      <c r="C30">
+        <v>34.047626106194897</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>37.553020134228184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.67608297539200002</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1.1969999999999999E-3</v>
+      </c>
+      <c r="C31">
+        <v>21.994407821229</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>23.372598162071846</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.69183097091900003</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.913E-3</v>
+      </c>
+      <c r="C32">
+        <v>13.3511292460646</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>14.624673288029273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.70794578438400002</v>
+      </c>
+      <c r="B33" s="3">
+        <v>3.1199999999999999E-3</v>
+      </c>
+      <c r="C33">
+        <v>9.8155809523809694</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>8.9669871794871785</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.724435960075</v>
+      </c>
+      <c r="B34" s="3">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="C34">
+        <v>6.6434177165354296</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8285416666666672</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.74131024130099998</v>
+      </c>
+      <c r="B35" s="3">
+        <v>7.3400000000000002E-3</v>
+      </c>
+      <c r="C35">
+        <v>4.7964816666666703</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8115803814713893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>